<commit_message>
Correct pPDM for Miconia prasina
</commit_message>
<xml_diff>
--- a/data/RPE_DATA.xlsx
+++ b/data/RPE_DATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elena/Documents/EBD-PhD/R!/MS_JEcol_Resource-provisioning-effectiveness/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305901A4-8506-5640-A40C-8B6083346C7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64EBA4B-3D76-1348-9692-329CF93EAEF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29500" yWindow="-17220" windowWidth="33420" windowHeight="21320" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="10" r:id="rId1"/>
@@ -2451,7 +2451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -2995,8 +2995,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z297"/>
   <sheetViews>
-    <sheetView topLeftCell="A252" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA179" sqref="AA179:AA183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17718,9 +17719,9 @@
       <c r="O179" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="P179" s="49">
-        <f>0.75*N179</f>
-        <v>0.09</v>
+      <c r="P179" s="50">
+        <f>0.678*N179</f>
+        <v>8.1360000000000002E-2</v>
       </c>
       <c r="Q179" s="35"/>
       <c r="R179" s="13" t="s">
@@ -17743,7 +17744,7 @@
       </c>
       <c r="X179" s="10">
         <f>(35*S179+14.1*T179+15.1*U179)*P179</f>
-        <v>1.124811</v>
+        <v>1.0168291439999999</v>
       </c>
       <c r="Y179" s="37" t="e">
         <f>(35*S179+14.1*T179+15.1*V179)*Q179</f>
@@ -17799,9 +17800,9 @@
       <c r="O180" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="P180" s="49">
-        <f>0.75*N180</f>
-        <v>0.09</v>
+      <c r="P180" s="50">
+        <f t="shared" ref="P180:P181" si="19">0.678*N180</f>
+        <v>8.1360000000000002E-2</v>
       </c>
       <c r="Q180" s="35"/>
       <c r="R180" s="13" t="s">
@@ -17824,7 +17825,7 @@
       </c>
       <c r="X180" s="10">
         <f>(35*S180+14.1*T180+15.1*U180)*P180</f>
-        <v>1.124811</v>
+        <v>1.0168291439999999</v>
       </c>
       <c r="Y180" s="37" t="e">
         <f>(35*S180+14.1*T180+15.1*V180)*Q180</f>
@@ -17880,9 +17881,9 @@
       <c r="O181" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="P181" s="49">
-        <f>0.75*N181</f>
-        <v>0.09</v>
+      <c r="P181" s="50">
+        <f t="shared" si="19"/>
+        <v>8.1360000000000002E-2</v>
       </c>
       <c r="Q181" s="35"/>
       <c r="R181" s="13" t="s">
@@ -17905,7 +17906,7 @@
       </c>
       <c r="X181" s="10">
         <f>(35*S181+14.1*T181+15.1*U181)*P181</f>
-        <v>1.124811</v>
+        <v>1.0168291439999999</v>
       </c>
       <c r="Y181" s="37" t="e">
         <f>(35*S181+14.1*T181+15.1*V181)*Q181</f>
@@ -17986,11 +17987,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X182" s="10">
-        <f t="shared" ref="X182:X214" si="19">(35*S182+14.1*T182+15.1*W182)*P182</f>
+        <f t="shared" ref="X182:X214" si="20">(35*S182+14.1*T182+15.1*W182)*P182</f>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y182" s="37">
-        <f t="shared" ref="Y182:Y214" si="20">(35*S182+14.1*T182+15.1*W182)*Q182</f>
+        <f t="shared" ref="Y182:Y214" si="21">(35*S182+14.1*T182+15.1*W182)*Q182</f>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z182" s="13" t="s">
@@ -18068,11 +18069,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X183" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y183" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z183" s="13" t="s">
@@ -18150,11 +18151,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X184" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y184" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z184" s="13" t="s">
@@ -18232,11 +18233,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X185" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y185" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z185" s="13" t="s">
@@ -18314,11 +18315,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X186" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y186" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z186" s="13" t="s">
@@ -18396,11 +18397,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X187" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y187" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z187" s="13" t="s">
@@ -18478,11 +18479,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X188" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y188" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z188" s="13" t="s">
@@ -18560,11 +18561,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X189" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y189" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z189" s="13" t="s">
@@ -18642,11 +18643,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X190" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y190" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z190" s="13" t="s">
@@ -18724,11 +18725,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X191" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y191" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z191" s="13" t="s">
@@ -18806,11 +18807,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X192" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y192" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z192" s="13" t="s">
@@ -18888,11 +18889,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X193" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y193" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z193" s="13" t="s">
@@ -18970,11 +18971,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X194" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y194" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z194" s="13" t="s">
@@ -19052,11 +19053,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X195" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y195" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z195" s="13" t="s">
@@ -19134,11 +19135,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X196" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y196" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z196" s="13" t="s">
@@ -19216,11 +19217,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X197" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y197" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z197" s="13" t="s">
@@ -19298,11 +19299,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X198" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y198" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z198" s="13" t="s">
@@ -19380,11 +19381,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X199" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y199" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z199" s="13" t="s">
@@ -19462,11 +19463,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X200" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y200" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z200" s="13" t="s">
@@ -19544,11 +19545,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X201" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y201" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z201" s="13" t="s">
@@ -19626,11 +19627,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X202" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y202" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z202" s="13" t="s">
@@ -19708,11 +19709,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X203" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y203" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z203" s="13" t="s">
@@ -19790,11 +19791,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X204" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y204" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z204" s="13" t="s">
@@ -19872,11 +19873,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X205" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y205" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z205" s="13" t="s">
@@ -19954,11 +19955,11 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="X206" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25090519999999999</v>
       </c>
       <c r="Y206" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.7720184863791777E-2</v>
       </c>
       <c r="Z206" s="13" t="s">
@@ -20036,11 +20037,11 @@
         <v>0.14899999999999999</v>
       </c>
       <c r="X207" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.16904579999999997</v>
       </c>
       <c r="Y207" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2.6960846846432698E-2</v>
       </c>
       <c r="Z207" s="13" t="s">
@@ -20118,11 +20119,11 @@
         <v>0.14899999999999999</v>
       </c>
       <c r="X208" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.16904579999999997</v>
       </c>
       <c r="Y208" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2.6960846846432698E-2</v>
       </c>
       <c r="Z208" s="13" t="s">
@@ -20200,11 +20201,11 @@
         <v>1E-3</v>
       </c>
       <c r="X209" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.5792000000000002E-2</v>
       </c>
       <c r="Y209" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.1312194358710944E-2</v>
       </c>
       <c r="Z209" s="13" t="s">
@@ -20282,11 +20283,11 @@
         <v>1E-3</v>
       </c>
       <c r="X210" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.5792000000000002E-2</v>
       </c>
       <c r="Y210" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.1312194358710944E-2</v>
       </c>
       <c r="Z210" s="13" t="s">
@@ -20364,11 +20365,11 @@
         <v>1E-3</v>
       </c>
       <c r="X211" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.5792000000000002E-2</v>
       </c>
       <c r="Y211" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.1312194358710944E-2</v>
       </c>
       <c r="Z211" s="13" t="s">
@@ -20446,11 +20447,11 @@
         <v>1E-3</v>
       </c>
       <c r="X212" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.5792000000000002E-2</v>
       </c>
       <c r="Y212" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.1312194358710944E-2</v>
       </c>
       <c r="Z212" s="13" t="s">
@@ -20528,11 +20529,11 @@
         <v>1E-3</v>
       </c>
       <c r="X213" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.5792000000000002E-2</v>
       </c>
       <c r="Y213" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.1312194358710944E-2</v>
       </c>
       <c r="Z213" s="13" t="s">
@@ -20610,11 +20611,11 @@
         <v>1E-3</v>
       </c>
       <c r="X214" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.5792000000000002E-2</v>
       </c>
       <c r="Y214" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.1312194358710944E-2</v>
       </c>
       <c r="Z214" s="13" t="s">
@@ -20665,11 +20666,11 @@
         <v>0.33</v>
       </c>
       <c r="O215" s="49">
-        <f t="shared" ref="O215:O220" si="21">0.527*N215</f>
+        <f t="shared" ref="O215:O220" si="22">0.527*N215</f>
         <v>0.17391000000000001</v>
       </c>
       <c r="P215" s="49">
-        <f t="shared" ref="P215:P220" si="22">O215*(1-R215)</f>
+        <f t="shared" ref="P215:P220" si="23">O215*(1-R215)</f>
         <v>7.6520399999999988E-2</v>
       </c>
       <c r="Q215" s="35">
@@ -20694,11 +20695,11 @@
         <v>23</v>
       </c>
       <c r="X215" s="10">
-        <f t="shared" ref="X215:X220" si="23">(35*S215+14.1*T215+15.1*U215)*P215</f>
+        <f t="shared" ref="X215:X220" si="24">(35*S215+14.1*T215+15.1*U215)*P215</f>
         <v>1.9260873363599995</v>
       </c>
       <c r="Y215" s="37">
-        <f t="shared" ref="Y215:Y220" si="24">(35*S215+14.1*T215+15.1*U215)*Q215</f>
+        <f t="shared" ref="Y215:Y220" si="25">(35*S215+14.1*T215+15.1*U215)*Q215</f>
         <v>0.52529654628000022</v>
       </c>
       <c r="Z215" s="13" t="s">
@@ -20749,11 +20750,11 @@
         <v>0.33</v>
       </c>
       <c r="O216" s="49">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.17391000000000001</v>
       </c>
       <c r="P216" s="49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>7.6520399999999988E-2</v>
       </c>
       <c r="Q216" s="35">
@@ -20778,11 +20779,11 @@
         <v>23</v>
       </c>
       <c r="X216" s="10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1.9260873363599995</v>
       </c>
       <c r="Y216" s="37">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.52529654628000022</v>
       </c>
       <c r="Z216" s="13" t="s">
@@ -20833,11 +20834,11 @@
         <v>0.33</v>
       </c>
       <c r="O217" s="49">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.17391000000000001</v>
       </c>
       <c r="P217" s="49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>7.6520399999999988E-2</v>
       </c>
       <c r="Q217" s="35">
@@ -20862,11 +20863,11 @@
         <v>23</v>
       </c>
       <c r="X217" s="10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1.9260873363599995</v>
       </c>
       <c r="Y217" s="37">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.52529654628000022</v>
       </c>
       <c r="Z217" s="13" t="s">
@@ -20917,11 +20918,11 @@
         <v>0.33</v>
       </c>
       <c r="O218" s="49">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.17391000000000001</v>
       </c>
       <c r="P218" s="49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>7.6520399999999988E-2</v>
       </c>
       <c r="Q218" s="35">
@@ -20946,11 +20947,11 @@
         <v>23</v>
       </c>
       <c r="X218" s="10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1.9260873363599995</v>
       </c>
       <c r="Y218" s="37">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.52529654628000022</v>
       </c>
       <c r="Z218" s="13" t="s">
@@ -21001,11 +21002,11 @@
         <v>0.33</v>
       </c>
       <c r="O219" s="49">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.17391000000000001</v>
       </c>
       <c r="P219" s="49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>7.6520399999999988E-2</v>
       </c>
       <c r="Q219" s="35">
@@ -21030,11 +21031,11 @@
         <v>23</v>
       </c>
       <c r="X219" s="10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1.9260873363599995</v>
       </c>
       <c r="Y219" s="37">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.52529654628000022</v>
       </c>
       <c r="Z219" s="13" t="s">
@@ -21085,11 +21086,11 @@
         <v>0.33</v>
       </c>
       <c r="O220" s="49">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.17391000000000001</v>
       </c>
       <c r="P220" s="49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>7.6520399999999988E-2</v>
       </c>
       <c r="Q220" s="35">
@@ -21114,11 +21115,11 @@
         <v>23</v>
       </c>
       <c r="X220" s="10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1.9260873363599995</v>
       </c>
       <c r="Y220" s="37">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.52529654628000022</v>
       </c>
       <c r="Z220" s="13" t="s">
@@ -21356,7 +21357,7 @@
         <v>23</v>
       </c>
       <c r="X223" s="51">
-        <f t="shared" ref="X223:X226" si="25">P223*21.045</f>
+        <f t="shared" ref="X223:X226" si="26">P223*21.045</f>
         <v>0.1536285</v>
       </c>
       <c r="Y223" s="50">
@@ -21436,7 +21437,7 @@
         <v>23</v>
       </c>
       <c r="X224" s="51">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.1536285</v>
       </c>
       <c r="Y224" s="50">
@@ -21516,7 +21517,7 @@
         <v>23</v>
       </c>
       <c r="X225" s="51">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.1536285</v>
       </c>
       <c r="Y225" s="50">
@@ -21596,7 +21597,7 @@
         <v>23</v>
       </c>
       <c r="X226" s="51">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.1536285</v>
       </c>
       <c r="Y226" s="50">
@@ -21682,7 +21683,7 @@
         <v>4.2033384000000007</v>
       </c>
       <c r="Y227" s="37">
-        <f t="shared" ref="Y227:Y238" si="26">(35*S227+14.1*T227+15.1*W227)*Q227</f>
+        <f t="shared" ref="Y227:Y238" si="27">(35*S227+14.1*T227+15.1*W227)*Q227</f>
         <v>1.7289548799999999</v>
       </c>
       <c r="Z227" s="13" t="s">
@@ -21760,11 +21761,11 @@
         <v>1.4E-2</v>
       </c>
       <c r="X228" s="10">
-        <f t="shared" ref="X228:X238" si="27">(35*S228+14.1*T228+15.1*W228)*P228</f>
+        <f t="shared" ref="X228:X238" si="28">(35*S228+14.1*T228+15.1*W228)*P228</f>
         <v>4.2033384000000007</v>
       </c>
       <c r="Y228" s="37">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1.7289548799999999</v>
       </c>
       <c r="Z228" s="13" t="s">
@@ -21842,11 +21843,11 @@
         <v>1.4E-2</v>
       </c>
       <c r="X229" s="10">
+        <f t="shared" si="28"/>
+        <v>4.2033384000000007</v>
+      </c>
+      <c r="Y229" s="37">
         <f t="shared" si="27"/>
-        <v>4.2033384000000007</v>
-      </c>
-      <c r="Y229" s="37">
-        <f t="shared" si="26"/>
         <v>1.7289548799999999</v>
       </c>
       <c r="Z229" s="13" t="s">
@@ -21924,11 +21925,11 @@
         <v>1.4E-2</v>
       </c>
       <c r="X230" s="10">
+        <f t="shared" si="28"/>
+        <v>4.2033384000000007</v>
+      </c>
+      <c r="Y230" s="37">
         <f t="shared" si="27"/>
-        <v>4.2033384000000007</v>
-      </c>
-      <c r="Y230" s="37">
-        <f t="shared" si="26"/>
         <v>1.7289548799999999</v>
       </c>
       <c r="Z230" s="13" t="s">
@@ -22007,11 +22008,11 @@
         <v>1.4E-2</v>
       </c>
       <c r="X231" s="10">
+        <f t="shared" si="28"/>
+        <v>4.2033384000000007</v>
+      </c>
+      <c r="Y231" s="37">
         <f t="shared" si="27"/>
-        <v>4.2033384000000007</v>
-      </c>
-      <c r="Y231" s="37">
-        <f t="shared" si="26"/>
         <v>1.7289548799999999</v>
       </c>
       <c r="Z231" s="13" t="s">
@@ -22089,11 +22090,11 @@
         <v>1.4E-2</v>
       </c>
       <c r="X232" s="10">
+        <f t="shared" si="28"/>
+        <v>4.2033384000000007</v>
+      </c>
+      <c r="Y232" s="37">
         <f t="shared" si="27"/>
-        <v>4.2033384000000007</v>
-      </c>
-      <c r="Y232" s="37">
-        <f t="shared" si="26"/>
         <v>1.7289548799999999</v>
       </c>
       <c r="Z232" s="13" t="s">
@@ -22171,11 +22172,11 @@
         <v>1.4E-2</v>
       </c>
       <c r="X233" s="10">
+        <f t="shared" si="28"/>
+        <v>4.2033384000000007</v>
+      </c>
+      <c r="Y233" s="37">
         <f t="shared" si="27"/>
-        <v>4.2033384000000007</v>
-      </c>
-      <c r="Y233" s="37">
-        <f t="shared" si="26"/>
         <v>1.7289548799999999</v>
       </c>
       <c r="Z233" s="13" t="s">
@@ -22253,11 +22254,11 @@
         <v>1.4E-2</v>
       </c>
       <c r="X234" s="10">
+        <f t="shared" si="28"/>
+        <v>4.2033384000000007</v>
+      </c>
+      <c r="Y234" s="37">
         <f t="shared" si="27"/>
-        <v>4.2033384000000007</v>
-      </c>
-      <c r="Y234" s="37">
-        <f t="shared" si="26"/>
         <v>1.7289548799999999</v>
       </c>
       <c r="Z234" s="13" t="s">
@@ -22335,11 +22336,11 @@
         <v>1.4E-2</v>
       </c>
       <c r="X235" s="10">
+        <f t="shared" si="28"/>
+        <v>4.2033384000000007</v>
+      </c>
+      <c r="Y235" s="37">
         <f t="shared" si="27"/>
-        <v>4.2033384000000007</v>
-      </c>
-      <c r="Y235" s="37">
-        <f t="shared" si="26"/>
         <v>1.7289548799999999</v>
       </c>
       <c r="Z235" s="13" t="s">
@@ -22417,11 +22418,11 @@
         <v>1.4E-2</v>
       </c>
       <c r="X236" s="10">
+        <f t="shared" si="28"/>
+        <v>4.2033384000000007</v>
+      </c>
+      <c r="Y236" s="37">
         <f t="shared" si="27"/>
-        <v>4.2033384000000007</v>
-      </c>
-      <c r="Y236" s="37">
-        <f t="shared" si="26"/>
         <v>1.7289548799999999</v>
       </c>
       <c r="Z236" s="13" t="s">
@@ -22499,11 +22500,11 @@
         <v>1.4E-2</v>
       </c>
       <c r="X237" s="10">
+        <f t="shared" si="28"/>
+        <v>4.2033384000000007</v>
+      </c>
+      <c r="Y237" s="37">
         <f t="shared" si="27"/>
-        <v>4.2033384000000007</v>
-      </c>
-      <c r="Y237" s="37">
-        <f t="shared" si="26"/>
         <v>1.7289548799999999</v>
       </c>
       <c r="Z237" s="13" t="s">
@@ -22581,11 +22582,11 @@
         <v>1.4E-2</v>
       </c>
       <c r="X238" s="10">
+        <f t="shared" si="28"/>
+        <v>4.2033384000000007</v>
+      </c>
+      <c r="Y238" s="37">
         <f t="shared" si="27"/>
-        <v>4.2033384000000007</v>
-      </c>
-      <c r="Y238" s="37">
-        <f t="shared" si="26"/>
         <v>1.7289548799999999</v>
       </c>
       <c r="Z238" s="13" t="s">
@@ -22663,11 +22664,11 @@
         <v>23</v>
       </c>
       <c r="X239" s="10">
-        <f t="shared" ref="X239:X245" si="28">(35*S239+14.1*T239+15.1*U239)*P239</f>
+        <f t="shared" ref="X239:X245" si="29">(35*S239+14.1*T239+15.1*U239)*P239</f>
         <v>1.87775</v>
       </c>
       <c r="Y239" s="37">
-        <f t="shared" ref="Y239:Y245" si="29">(35*S239+14.1*T239+15.1*U239)*Q239</f>
+        <f t="shared" ref="Y239:Y245" si="30">(35*S239+14.1*T239+15.1*U239)*Q239</f>
         <v>0.19514840625000004</v>
       </c>
       <c r="Z239" s="13" t="s">
@@ -22745,11 +22746,11 @@
         <v>23</v>
       </c>
       <c r="X240" s="10">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.87775</v>
       </c>
       <c r="Y240" s="37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.19514840625000004</v>
       </c>
       <c r="Z240" s="13" t="s">
@@ -22827,11 +22828,11 @@
         <v>23</v>
       </c>
       <c r="X241" s="10">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.87775</v>
       </c>
       <c r="Y241" s="37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.19514840625000004</v>
       </c>
       <c r="Z241" s="13" t="s">
@@ -22909,11 +22910,11 @@
         <v>23</v>
       </c>
       <c r="X242" s="10">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.87775</v>
       </c>
       <c r="Y242" s="37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.19514840625000004</v>
       </c>
       <c r="Z242" s="13" t="s">
@@ -22991,11 +22992,11 @@
         <v>23</v>
       </c>
       <c r="X243" s="10">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.87775</v>
       </c>
       <c r="Y243" s="37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.19514840625000004</v>
       </c>
       <c r="Z243" s="13" t="s">
@@ -23073,11 +23074,11 @@
         <v>23</v>
       </c>
       <c r="X244" s="10">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.87775</v>
       </c>
       <c r="Y244" s="37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.19514840625000004</v>
       </c>
       <c r="Z244" s="13" t="s">
@@ -23155,11 +23156,11 @@
         <v>23</v>
       </c>
       <c r="X245" s="10">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.87775</v>
       </c>
       <c r="Y245" s="37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.19514840625000004</v>
       </c>
       <c r="Z245" s="13" t="s">
@@ -23241,7 +23242,7 @@
         <v>2.1236599999999998E-2</v>
       </c>
       <c r="Y246" s="37">
-        <f t="shared" ref="Y246:Y257" si="30">(35*S246+14.1*T246+15.1*W246)*Q246</f>
+        <f t="shared" ref="Y246:Y257" si="31">(35*S246+14.1*T246+15.1*W246)*Q246</f>
         <v>7.4370573199999948E-3</v>
       </c>
       <c r="Z246" s="13" t="s">
@@ -23319,11 +23320,11 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="X247" s="10">
-        <f t="shared" ref="X247:X257" si="31">(35*S247+14.1*T247+15.1*W247)*P247</f>
+        <f t="shared" ref="X247:X257" si="32">(35*S247+14.1*T247+15.1*W247)*P247</f>
         <v>2.1236599999999998E-2</v>
       </c>
       <c r="Y247" s="37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>7.4370573199999948E-3</v>
       </c>
       <c r="Z247" s="13" t="s">
@@ -23401,11 +23402,11 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="X248" s="10">
+        <f t="shared" si="32"/>
+        <v>2.1236599999999998E-2</v>
+      </c>
+      <c r="Y248" s="37">
         <f t="shared" si="31"/>
-        <v>2.1236599999999998E-2</v>
-      </c>
-      <c r="Y248" s="37">
-        <f t="shared" si="30"/>
         <v>7.4370573199999948E-3</v>
       </c>
       <c r="Z248" s="13" t="s">
@@ -23483,11 +23484,11 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="X249" s="10">
+        <f t="shared" si="32"/>
+        <v>2.1236599999999998E-2</v>
+      </c>
+      <c r="Y249" s="37">
         <f t="shared" si="31"/>
-        <v>2.1236599999999998E-2</v>
-      </c>
-      <c r="Y249" s="37">
-        <f t="shared" si="30"/>
         <v>7.4370573199999948E-3</v>
       </c>
       <c r="Z249" s="13" t="s">
@@ -23565,11 +23566,11 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="X250" s="10">
+        <f t="shared" si="32"/>
+        <v>2.1236599999999998E-2</v>
+      </c>
+      <c r="Y250" s="37">
         <f t="shared" si="31"/>
-        <v>2.1236599999999998E-2</v>
-      </c>
-      <c r="Y250" s="37">
-        <f t="shared" si="30"/>
         <v>7.4370573199999948E-3</v>
       </c>
       <c r="Z250" s="13" t="s">
@@ -23647,11 +23648,11 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="X251" s="10">
+        <f t="shared" si="32"/>
+        <v>2.1236599999999998E-2</v>
+      </c>
+      <c r="Y251" s="37">
         <f t="shared" si="31"/>
-        <v>2.1236599999999998E-2</v>
-      </c>
-      <c r="Y251" s="37">
-        <f t="shared" si="30"/>
         <v>7.4370573199999948E-3</v>
       </c>
       <c r="Z251" s="13" t="s">
@@ -23729,11 +23730,11 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="X252" s="10">
+        <f t="shared" si="32"/>
+        <v>2.1236599999999998E-2</v>
+      </c>
+      <c r="Y252" s="37">
         <f t="shared" si="31"/>
-        <v>2.1236599999999998E-2</v>
-      </c>
-      <c r="Y252" s="37">
-        <f t="shared" si="30"/>
         <v>7.4370573199999948E-3</v>
       </c>
       <c r="Z252" s="13" t="s">
@@ -23811,11 +23812,11 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="X253" s="10">
+        <f t="shared" si="32"/>
+        <v>2.1236599999999998E-2</v>
+      </c>
+      <c r="Y253" s="37">
         <f t="shared" si="31"/>
-        <v>2.1236599999999998E-2</v>
-      </c>
-      <c r="Y253" s="37">
-        <f t="shared" si="30"/>
         <v>7.4370573199999948E-3</v>
       </c>
       <c r="Z253" s="13" t="s">
@@ -23893,11 +23894,11 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="X254" s="10">
+        <f t="shared" si="32"/>
+        <v>2.1236599999999998E-2</v>
+      </c>
+      <c r="Y254" s="37">
         <f t="shared" si="31"/>
-        <v>2.1236599999999998E-2</v>
-      </c>
-      <c r="Y254" s="37">
-        <f t="shared" si="30"/>
         <v>7.4370573199999948E-3</v>
       </c>
       <c r="Z254" s="13" t="s">
@@ -23975,11 +23976,11 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="X255" s="10">
+        <f t="shared" si="32"/>
+        <v>2.1236599999999998E-2</v>
+      </c>
+      <c r="Y255" s="37">
         <f t="shared" si="31"/>
-        <v>2.1236599999999998E-2</v>
-      </c>
-      <c r="Y255" s="37">
-        <f t="shared" si="30"/>
         <v>7.4370573199999948E-3</v>
       </c>
       <c r="Z255" s="13" t="s">
@@ -24057,11 +24058,11 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="X256" s="10">
+        <f t="shared" si="32"/>
+        <v>2.1236599999999998E-2</v>
+      </c>
+      <c r="Y256" s="37">
         <f t="shared" si="31"/>
-        <v>2.1236599999999998E-2</v>
-      </c>
-      <c r="Y256" s="37">
-        <f t="shared" si="30"/>
         <v>7.4370573199999948E-3</v>
       </c>
       <c r="Z256" s="13" t="s">
@@ -24139,11 +24140,11 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="X257" s="10">
+        <f t="shared" si="32"/>
+        <v>2.1236599999999998E-2</v>
+      </c>
+      <c r="Y257" s="37">
         <f t="shared" si="31"/>
-        <v>2.1236599999999998E-2</v>
-      </c>
-      <c r="Y257" s="37">
-        <f t="shared" si="30"/>
         <v>7.4370573199999948E-3</v>
       </c>
       <c r="Z257" s="13" t="s">
@@ -24303,7 +24304,7 @@
         <v>23</v>
       </c>
       <c r="X259" s="10">
-        <f t="shared" ref="X259:X264" si="32">(35*S259+14.1*T259+15.1*V259)*P259</f>
+        <f t="shared" ref="X259:X264" si="33">(35*S259+14.1*T259+15.1*V259)*P259</f>
         <v>2.7512089241278357</v>
       </c>
       <c r="Y259" s="37">
@@ -24385,7 +24386,7 @@
         <v>23</v>
       </c>
       <c r="X260" s="10">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.7512089241278357</v>
       </c>
       <c r="Y260" s="37">
@@ -24467,7 +24468,7 @@
         <v>23</v>
       </c>
       <c r="X261" s="10">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.7512089241278357</v>
       </c>
       <c r="Y261" s="37">
@@ -24549,7 +24550,7 @@
         <v>23</v>
       </c>
       <c r="X262" s="10">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>4.4800359999999992</v>
       </c>
       <c r="Y262" s="35" t="s">
@@ -24631,7 +24632,7 @@
         <v>23</v>
       </c>
       <c r="X263" s="10">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>4.4800359999999992</v>
       </c>
       <c r="Y263" s="35" t="s">
@@ -24712,7 +24713,7 @@
         <v>23</v>
       </c>
       <c r="X264" s="10">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>4.4800359999999992</v>
       </c>
       <c r="Y264" s="35" t="s">
@@ -25202,7 +25203,7 @@
         <v>0.1135254</v>
       </c>
       <c r="Y270" s="37">
-        <f t="shared" ref="Y270:Y283" si="33">(35*S270+14.1*T270+15.1*W270)*Q270</f>
+        <f t="shared" ref="Y270:Y283" si="34">(35*S270+14.1*T270+15.1*W270)*Q270</f>
         <v>2.5769281913199989E-2</v>
       </c>
       <c r="Z270" s="13" t="s">
@@ -25280,11 +25281,11 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="X271" s="10">
-        <f t="shared" ref="X271:X283" si="34">(35*S271+14.1*T271+15.1*W271)*P271</f>
+        <f t="shared" ref="X271:X283" si="35">(35*S271+14.1*T271+15.1*W271)*P271</f>
         <v>0.1135254</v>
       </c>
       <c r="Y271" s="37">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>2.5769281913199989E-2</v>
       </c>
       <c r="Z271" s="13" t="s">
@@ -25362,11 +25363,11 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="X272" s="10">
+        <f t="shared" si="35"/>
+        <v>0.1135254</v>
+      </c>
+      <c r="Y272" s="37">
         <f t="shared" si="34"/>
-        <v>0.1135254</v>
-      </c>
-      <c r="Y272" s="37">
-        <f t="shared" si="33"/>
         <v>2.5769281913199989E-2</v>
       </c>
       <c r="Z272" s="13" t="s">
@@ -25444,11 +25445,11 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="X273" s="10">
+        <f t="shared" si="35"/>
+        <v>0.1135254</v>
+      </c>
+      <c r="Y273" s="37">
         <f t="shared" si="34"/>
-        <v>0.1135254</v>
-      </c>
-      <c r="Y273" s="37">
-        <f t="shared" si="33"/>
         <v>2.5769281913199989E-2</v>
       </c>
       <c r="Z273" s="13" t="s">
@@ -25526,11 +25527,11 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="X274" s="10">
+        <f t="shared" si="35"/>
+        <v>0.1135254</v>
+      </c>
+      <c r="Y274" s="37">
         <f t="shared" si="34"/>
-        <v>0.1135254</v>
-      </c>
-      <c r="Y274" s="37">
-        <f t="shared" si="33"/>
         <v>2.5769281913199989E-2</v>
       </c>
       <c r="Z274" s="13" t="s">
@@ -25608,11 +25609,11 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="X275" s="10">
+        <f t="shared" si="35"/>
+        <v>0.1135254</v>
+      </c>
+      <c r="Y275" s="37">
         <f t="shared" si="34"/>
-        <v>0.1135254</v>
-      </c>
-      <c r="Y275" s="37">
-        <f t="shared" si="33"/>
         <v>2.5769281913199989E-2</v>
       </c>
       <c r="Z275" s="13" t="s">
@@ -25690,11 +25691,11 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="X276" s="10">
+        <f t="shared" si="35"/>
+        <v>0.1135254</v>
+      </c>
+      <c r="Y276" s="37">
         <f t="shared" si="34"/>
-        <v>0.1135254</v>
-      </c>
-      <c r="Y276" s="37">
-        <f t="shared" si="33"/>
         <v>2.5769281913199989E-2</v>
       </c>
       <c r="Z276" s="13" t="s">
@@ -25772,11 +25773,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="X277" s="10">
+        <f t="shared" si="35"/>
+        <v>14.722417999999999</v>
+      </c>
+      <c r="Y277" s="37">
         <f t="shared" si="34"/>
-        <v>14.722417999999999</v>
-      </c>
-      <c r="Y277" s="37">
-        <f t="shared" si="33"/>
         <v>0.68842856000000008</v>
       </c>
       <c r="Z277" s="13" t="s">
@@ -25854,11 +25855,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="X278" s="10">
+        <f t="shared" si="35"/>
+        <v>14.722417999999999</v>
+      </c>
+      <c r="Y278" s="37">
         <f t="shared" si="34"/>
-        <v>14.722417999999999</v>
-      </c>
-      <c r="Y278" s="37">
-        <f t="shared" si="33"/>
         <v>0.68842856000000008</v>
       </c>
       <c r="Z278" s="13" t="s">
@@ -25936,11 +25937,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="X279" s="10">
+        <f t="shared" si="35"/>
+        <v>14.722417999999999</v>
+      </c>
+      <c r="Y279" s="37">
         <f t="shared" si="34"/>
-        <v>14.722417999999999</v>
-      </c>
-      <c r="Y279" s="37">
-        <f t="shared" si="33"/>
         <v>0.68842856000000008</v>
       </c>
       <c r="Z279" s="13" t="s">
@@ -26018,11 +26019,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="X280" s="10">
+        <f t="shared" si="35"/>
+        <v>14.722417999999999</v>
+      </c>
+      <c r="Y280" s="37">
         <f t="shared" si="34"/>
-        <v>14.722417999999999</v>
-      </c>
-      <c r="Y280" s="37">
-        <f t="shared" si="33"/>
         <v>0.68842856000000008</v>
       </c>
       <c r="Z280" s="13" t="s">
@@ -26100,11 +26101,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="X281" s="10">
+        <f t="shared" si="35"/>
+        <v>14.722417999999999</v>
+      </c>
+      <c r="Y281" s="37">
         <f t="shared" si="34"/>
-        <v>14.722417999999999</v>
-      </c>
-      <c r="Y281" s="37">
-        <f t="shared" si="33"/>
         <v>0.68842856000000008</v>
       </c>
       <c r="Z281" s="13" t="s">
@@ -26182,11 +26183,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="X282" s="10">
+        <f t="shared" si="35"/>
+        <v>14.722417999999999</v>
+      </c>
+      <c r="Y282" s="37">
         <f t="shared" si="34"/>
-        <v>14.722417999999999</v>
-      </c>
-      <c r="Y282" s="37">
-        <f t="shared" si="33"/>
         <v>0.68842856000000008</v>
       </c>
       <c r="Z282" s="13" t="s">
@@ -26264,11 +26265,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="X283" s="10">
+        <f t="shared" si="35"/>
+        <v>14.722417999999999</v>
+      </c>
+      <c r="Y283" s="37">
         <f t="shared" si="34"/>
-        <v>14.722417999999999</v>
-      </c>
-      <c r="Y283" s="37">
-        <f t="shared" si="33"/>
         <v>0.68842856000000008</v>
       </c>
       <c r="Z283" s="13" t="s">
@@ -26322,7 +26323,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="P284" s="48">
-        <f t="shared" ref="P284:P290" si="35">O284*(1-R284)</f>
+        <f t="shared" ref="P284:P290" si="36">O284*(1-R284)</f>
         <v>0.40700000000000003</v>
       </c>
       <c r="Q284" s="35">
@@ -26351,7 +26352,7 @@
         <v>11.040159900000001</v>
       </c>
       <c r="Y284" s="37">
-        <f t="shared" ref="Y284:Y290" si="36">(35*S284+14.1*T284+15.1*V284)*Q284</f>
+        <f t="shared" ref="Y284:Y290" si="37">(35*S284+14.1*T284+15.1*V284)*Q284</f>
         <v>0.5018254499999999</v>
       </c>
       <c r="Z284" s="13" t="s">
@@ -26405,7 +26406,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="P285" s="48">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.40700000000000003</v>
       </c>
       <c r="Q285" s="35">
@@ -26430,11 +26431,11 @@
         <v>23</v>
       </c>
       <c r="X285" s="10">
-        <f t="shared" ref="X285:X290" si="37">(35*S285+14.1*T285+15.1*V285)*P285</f>
+        <f t="shared" ref="X285:X290" si="38">(35*S285+14.1*T285+15.1*V285)*P285</f>
         <v>11.040159900000001</v>
       </c>
       <c r="Y285" s="37">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0.5018254499999999</v>
       </c>
       <c r="Z285" s="13" t="s">
@@ -26489,7 +26490,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="P286" s="48">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.40700000000000003</v>
       </c>
       <c r="Q286" s="35">
@@ -26514,11 +26515,11 @@
         <v>23</v>
       </c>
       <c r="X286" s="10">
+        <f t="shared" si="38"/>
+        <v>11.040159900000001</v>
+      </c>
+      <c r="Y286" s="37">
         <f t="shared" si="37"/>
-        <v>11.040159900000001</v>
-      </c>
-      <c r="Y286" s="37">
-        <f t="shared" si="36"/>
         <v>0.5018254499999999</v>
       </c>
       <c r="Z286" s="13" t="s">
@@ -26572,7 +26573,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="P287" s="48">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.40700000000000003</v>
       </c>
       <c r="Q287" s="35">
@@ -26597,11 +26598,11 @@
         <v>23</v>
       </c>
       <c r="X287" s="10">
+        <f t="shared" si="38"/>
+        <v>11.040159900000001</v>
+      </c>
+      <c r="Y287" s="37">
         <f t="shared" si="37"/>
-        <v>11.040159900000001</v>
-      </c>
-      <c r="Y287" s="37">
-        <f t="shared" si="36"/>
         <v>0.5018254499999999</v>
       </c>
       <c r="Z287" s="13" t="s">
@@ -26655,7 +26656,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="P288" s="48">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.40700000000000003</v>
       </c>
       <c r="Q288" s="35">
@@ -26680,11 +26681,11 @@
         <v>23</v>
       </c>
       <c r="X288" s="10">
+        <f t="shared" si="38"/>
+        <v>11.040159900000001</v>
+      </c>
+      <c r="Y288" s="37">
         <f t="shared" si="37"/>
-        <v>11.040159900000001</v>
-      </c>
-      <c r="Y288" s="37">
-        <f t="shared" si="36"/>
         <v>0.5018254499999999</v>
       </c>
       <c r="Z288" s="13" t="s">
@@ -26738,7 +26739,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="P289" s="48">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.40700000000000003</v>
       </c>
       <c r="Q289" s="35">
@@ -26763,11 +26764,11 @@
         <v>23</v>
       </c>
       <c r="X289" s="10">
+        <f t="shared" si="38"/>
+        <v>11.040159900000001</v>
+      </c>
+      <c r="Y289" s="37">
         <f t="shared" si="37"/>
-        <v>11.040159900000001</v>
-      </c>
-      <c r="Y289" s="37">
-        <f t="shared" si="36"/>
         <v>0.5018254499999999</v>
       </c>
       <c r="Z289" s="13" t="s">
@@ -26821,7 +26822,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="P290" s="48">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.40700000000000003</v>
       </c>
       <c r="Q290" s="35">
@@ -26846,11 +26847,11 @@
         <v>23</v>
       </c>
       <c r="X290" s="10">
+        <f t="shared" si="38"/>
+        <v>11.040159900000001</v>
+      </c>
+      <c r="Y290" s="37">
         <f t="shared" si="37"/>
-        <v>11.040159900000001</v>
-      </c>
-      <c r="Y290" s="37">
-        <f t="shared" si="36"/>
         <v>0.5018254499999999</v>
       </c>
       <c r="Z290" s="13" t="s">
@@ -27439,8 +27440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Y121"/>
   <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Y1048576"/>
+    <sheetView topLeftCell="F1" zoomScale="86" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27569,7 +27570,7 @@
         <v>1.3637160000000002E-2</v>
       </c>
       <c r="G2" s="1">
-        <f t="shared" ref="G2:G37" si="0">AVERAGE(H2:Y2)</f>
+        <f>AVERAGE(H2:Y2)</f>
         <v>0.15531780326400002</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -27647,7 +27648,7 @@
         <v>4.5796094999999998E-3</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G2:G37" si="0">AVERAGE(H3:Y3)</f>
         <v>1.5739735059991666</v>
       </c>
       <c r="H3" s="1" t="s">

</xml_diff>